<commit_message>
I fixed most of the trendlines. The Log trendline still needs work.
</commit_message>
<xml_diff>
--- a/CurveFitting/Curve Fitting 2.xlsx
+++ b/CurveFitting/Curve Fitting 2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -39,18 +39,6 @@
     <t>Sumx^2</t>
   </si>
   <si>
-    <t>Solve for a &amp; b now.</t>
-  </si>
-  <si>
-    <t>Do y=A+B*x</t>
-  </si>
-  <si>
-    <t>a=</t>
-  </si>
-  <si>
-    <t>b=</t>
-  </si>
-  <si>
     <t>Solve the following system of equations in Excel, using the matrix inversion method:</t>
   </si>
   <si>
@@ -659,6 +647,18 @@
   </si>
   <si>
     <t>x4</t>
+  </si>
+  <si>
+    <t>Sumx^3</t>
+  </si>
+  <si>
+    <t>Sumx^4</t>
+  </si>
+  <si>
+    <t>Sumx^5</t>
+  </si>
+  <si>
+    <t>Sumx^6</t>
   </si>
 </sst>
 </file>
@@ -1042,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="H9:I9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,257 +1122,63 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <f>A2^2+A3^2+A4^2+A5^2</f>
+        <f>$A$2^F6+$A$3^F6+$A$4^F6+$A$5^F6</f>
         <v>9.7099999999999991</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <f>E2</f>
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <f>E3</f>
-        <v>5.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
       <c r="F9">
-        <f>E4</f>
-        <v>40.700000000000003</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <f>E3</f>
-        <v>5.5</v>
-      </c>
-      <c r="D10">
-        <f>E6</f>
-        <v>9.7099999999999991</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
+      <c r="D10" t="s">
+        <v>23</v>
       </c>
       <c r="F10">
-        <f>E5</f>
-        <v>59.78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <f>MINVERSE(C9:D10)</f>
-        <v>1.1303841676367872</v>
-      </c>
-      <c r="D12" t="e">
-        <f>MINVERSE(D9:E10)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="e">
-        <f>MINVERSE(C10:D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" t="e">
-        <f>MINVERSE(D10:E11)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="L22" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22">
-        <v>52.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>4</v>
-      </c>
-      <c r="J23">
-        <v>7</v>
-      </c>
-      <c r="M23">
-        <v>74.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
         <v>6</v>
       </c>
-      <c r="M24">
-        <v>58.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G25">
-        <v>3</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>3</v>
-      </c>
-      <c r="M25">
-        <v>34.200000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27">
-        <f t="array" ref="C27:F30">MINVERSE(G22:J25)</f>
-        <v>-0.11111111111111116</v>
-      </c>
-      <c r="D27">
-        <v>-0.1111111111111111</v>
-      </c>
-      <c r="E27">
-        <v>-0.11111111111111105</v>
-      </c>
-      <c r="F27">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="H27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27">
-        <f t="array" ref="I27:I30">MMULT(C27:F30,M22:M25)</f>
-        <v>2.2000000000000135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>-3.5555555555555562</v>
-      </c>
-      <c r="D28">
-        <v>-0.55555555555555547</v>
-      </c>
-      <c r="E28">
-        <v>1.4444444444444442</v>
-      </c>
-      <c r="F28">
-        <v>4.333333333333333</v>
-      </c>
-      <c r="H28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28">
-        <v>3.0999999999999659</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>-3.1111111111111112</v>
-      </c>
-      <c r="D29">
-        <v>-0.1111111111111111</v>
-      </c>
-      <c r="E29">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F29">
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29">
-        <v>4.4000000000000057</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>2.3333333333333335</v>
-      </c>
-      <c r="D30">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E30">
-        <v>-0.66666666666666663</v>
-      </c>
-      <c r="F30">
-        <v>-3</v>
-      </c>
-      <c r="H30" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30">
-        <v>6.7000000000000171</v>
-      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1391,23 +1197,23 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1422,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="M3">
         <v>52.9</v>
@@ -1430,7 +1236,7 @@
     </row>
     <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1450,7 +1256,7 @@
     </row>
     <row r="5" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -1487,7 +1293,7 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <f t="array" ref="C8:F11">MINVERSE(G3:J6)</f>
@@ -1503,7 +1309,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I8">
         <f t="array" ref="I8:I11">MMULT(C8:F11,M3:M6)</f>
@@ -1524,7 +1330,7 @@
         <v>4.333333333333333</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I9">
         <v>3.0999999999999659</v>
@@ -1544,7 +1350,7 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I10">
         <v>4.4000000000000057</v>
@@ -1564,7 +1370,7 @@
         <v>-3</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I11">
         <v>6.7000000000000171</v>

</xml_diff>